<commit_message>
Added Alert Exception when it does not exist and updated Sample spreadsheet with new commands and descriptions
</commit_message>
<xml_diff>
--- a/Samples/TestData/SampleTestSet2.xlsx
+++ b/Samples/TestData/SampleTestSet2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6225"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestSet" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
   <si>
     <t>Active</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Cleared!</t>
   </si>
   <si>
-    <t>What's up?</t>
-  </si>
-  <si>
     <t>alertButton1</t>
   </si>
   <si>
@@ -217,19 +214,112 @@
     <t>N</t>
   </si>
   <si>
-    <t>Alert accepted</t>
+    <t>Popup_JSAlert_GetText()</t>
   </si>
   <si>
-    <t>Confirm accepted</t>
+    <t>Popup_JSConfirm_GetText()</t>
   </si>
   <si>
-    <t>Confirm dismissed</t>
+    <t>Popup_JSPrompt_GetText()</t>
   </si>
   <si>
-    <t>Text typed</t>
+    <t>Hello!</t>
   </si>
   <si>
-    <t>Bye!</t>
+    <t>Ok or Cancel?</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Using MessageBox to pause</t>
+  </si>
+  <si>
+    <t>No Alert Present</t>
+  </si>
+  <si>
+    <t>Exception(s)</t>
+  </si>
+  <si>
+    <t>Tag of element. Ex: div</t>
+  </si>
+  <si>
+    <t>Name of html element. &lt;div name="theName"&gt;</t>
+  </si>
+  <si>
+    <t>Id of html element. &lt;div id="theId"&gt;</t>
+  </si>
+  <si>
+    <t>Class of html element. &lt;div class="theClass"&gt;</t>
+  </si>
+  <si>
+    <t>#node-55</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://"&gt;The link text&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>//*[@id="page-title"]</t>
+  </si>
+  <si>
+    <t>Clear, Click, MessageBox and Popup commands</t>
+  </si>
+  <si>
+    <t>Description or example</t>
+  </si>
+  <si>
+    <t>Clear the input</t>
+  </si>
+  <si>
+    <t>Perform a click</t>
+  </si>
+  <si>
+    <t>Send the inputStr text to the input</t>
+  </si>
+  <si>
+    <t>Submit form</t>
+  </si>
+  <si>
+    <t>Return True or False if element is displayed</t>
+  </si>
+  <si>
+    <t>Return True or False if element is enabled</t>
+  </si>
+  <si>
+    <t>Return True or False if element is selected</t>
+  </si>
+  <si>
+    <t>Return the atribute value for the specified attribute name. Exemple: href</t>
+  </si>
+  <si>
+    <t>Return the CSS value for the specified CSS property name. Example: color</t>
+  </si>
+  <si>
+    <t>Return the name of the html tag. Example: div</t>
+  </si>
+  <si>
+    <t>Return the inner Text of the html element. Example: &lt;span&gt;The inner text&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Navigate to the specified strURL</t>
+  </si>
+  <si>
+    <t>Close the window or browser</t>
+  </si>
+  <si>
+    <t>Return the text of the JS Alert</t>
+  </si>
+  <si>
+    <t>Click on Cancel of the JS Alert</t>
+  </si>
+  <si>
+    <t>Click on OK of the JS Alert</t>
+  </si>
+  <si>
+    <t>Send the inputStr text to the input of the JS Prompt Alert</t>
+  </si>
+  <si>
+    <t>Send the message to the screen. Can be used to pause execution.</t>
   </si>
 </sst>
 </file>
@@ -269,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +381,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -519,7 +615,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -856,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,7 +984,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -899,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -6683,7 +6782,7 @@
       <formula1>Commands!$A$2:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B499">
-      <formula1>Commands!$D$2:$D$10</formula1>
+      <formula1>Commands!$E$2:$E$10</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -6698,8 +6797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1359"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6790,12 +6889,12 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="17" t="str">
@@ -6805,17 +6904,17 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="G6" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>Passed</v>
+        <v>Failed</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6832,13 +6931,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6847,17 +6946,17 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="G9" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>Passed</v>
+        <v>Failed</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6874,13 +6973,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="G11" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6889,17 +6988,17 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="G12" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>Passed</v>
+        <v>Failed</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6916,13 +7015,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>68</v>
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="G14" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6931,17 +7030,17 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="7" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="G15" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>Passed</v>
+        <v>Failed</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6952,7 +7051,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G16" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6967,7 +7066,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G17" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6988,17 +7087,17 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>70</v>
+      <c r="F19" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="G19" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>Passed</v>
+        <v>Failed</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -12478,7 +12577,7 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B499">
-      <formula1>Commands!$D$2:$D$10</formula1>
+      <formula1>Commands!$E$2:$E$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A499">
       <formula1>Commands!$A$2:$A$30</formula1>
@@ -12494,185 +12593,307 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="66.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="E9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="B11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="B14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="B15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+      <c r="B20" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
+      <c r="B21" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>